<commit_message>
NetflixClone back doc update
</commit_message>
<xml_diff>
--- a/doc/Table_structure.xlsx
+++ b/doc/Table_structure.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrateur\Desktop\Projets\Netflix-Clone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrateur\Desktop\Projets\NetflixClone\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>User</t>
   </si>
@@ -44,12 +44,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>actif</t>
-  </si>
-  <si>
     <t>Faq</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
     <t>Image</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>url</t>
   </si>
   <si>
@@ -99,6 +90,21 @@
   </si>
   <si>
     <t>text</t>
+  </si>
+  <si>
+    <t>banned</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>role_id</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>size_type</t>
   </si>
 </sst>
 </file>
@@ -230,7 +236,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="37">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -255,13 +261,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
@@ -274,6 +273,13 @@
         </top>
         <bottom style="medium">
           <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
         </bottom>
       </border>
     </dxf>
@@ -334,13 +340,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
@@ -353,6 +352,13 @@
         </top>
         <bottom style="medium">
           <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
         </bottom>
       </border>
     </dxf>
@@ -413,13 +419,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
@@ -432,6 +431,13 @@
         </top>
         <bottom style="medium">
           <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
         </bottom>
       </border>
     </dxf>
@@ -492,13 +498,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
@@ -511,6 +510,13 @@
         </top>
         <bottom style="medium">
           <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
         </bottom>
       </border>
     </dxf>
@@ -549,67 +555,47 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
         <right style="medium">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
       <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
+        <bottom style="thin">
+          <color auto="1"/>
         </bottom>
       </border>
     </dxf>
@@ -670,13 +656,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color auto="1"/>
@@ -688,6 +667,13 @@
           <color auto="1"/>
         </top>
         <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
           <color auto="1"/>
         </bottom>
       </border>
@@ -710,6 +696,52 @@
       </font>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -725,6 +757,59 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -740,57 +825,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="C12:C16" totalsRowShown="0" headerRowDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="C12:C16" totalsRowShown="0" headerRowDxfId="36">
   <autoFilter ref="C12:C16"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Video" dataDxfId="20"/>
+    <tableColumn id="1" name="Video" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="C6:C10" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="23" tableBorderDxfId="24" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="C6:C10" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="C6:C10"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Image" dataDxfId="21"/>
+    <tableColumn id="1" name="Image" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau7" displayName="Tableau7" ref="C1:C4" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="28" tableBorderDxfId="29" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau7" displayName="Tableau7" ref="C1:C4" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="C1:C4"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Resource_Category" dataDxfId="26"/>
+    <tableColumn id="1" name="Resource_Category" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau8" displayName="Tableau8" ref="A19:A23" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3" totalsRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau8" displayName="Tableau8" ref="A19:A23" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="A19:A23"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Resource" dataDxfId="0"/>
+    <tableColumn id="1" name="Resource" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau9" displayName="Tableau9" ref="A15:A17" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau9" displayName="Tableau9" ref="A15:A17" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="A15:A17"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Category" dataDxfId="5"/>
+    <tableColumn id="1" name="Category" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau10" displayName="Tableau10" ref="A10:A13" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau10" displayName="Tableau10" ref="A10:A13" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A10:A13"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Faq" dataDxfId="10"/>
@@ -800,12 +885,22 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tableau11" displayName="Tableau11" ref="A1:A8" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tableau11" displayName="Tableau11" ref="A1:A8" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A1:A8"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="User" dataDxfId="15"/>
+    <tableColumn id="1" name="User" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau92" displayName="Tableau92" ref="C19:C21" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+  <autoFilter ref="C19:C21"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Role" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1075,7 +1170,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,15 +1184,15 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1105,7 +1200,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1113,7 +1208,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1126,114 +1221,123 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="7">
+  <pageSetup paperSize="11" orientation="portrait" r:id="rId1"/>
+  <tableParts count="8">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -1241,6 +1345,7 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
NetflixClone doc update : db structure
</commit_message>
<xml_diff>
--- a/doc/Table_structure.xlsx
+++ b/doc/Table_structure.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$C$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$C$26</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>User</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Resource</t>
   </si>
   <si>
-    <t>Resource_Category</t>
-  </si>
-  <si>
     <t>category_id</t>
   </si>
   <si>
@@ -105,6 +102,18 @@
   </si>
   <si>
     <t>size_type</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>genre_id</t>
+  </si>
+  <si>
+    <t>Genre_Resource</t>
+  </si>
+  <si>
+    <t>Category_Resource</t>
   </si>
 </sst>
 </file>
@@ -128,12 +137,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -222,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -232,57 +259,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="47">
     <dxf>
       <font>
         <b/>
@@ -299,7 +283,13 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -308,12 +298,36 @@
         </right>
         <top/>
         <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -333,31 +347,47 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="medium">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="medium">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
         <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
           <color auto="1"/>
         </bottom>
       </border>
@@ -378,22 +408,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -658,16 +672,16 @@
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="medium">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="medium">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
         <bottom style="medium">
-          <color auto="1"/>
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
@@ -694,6 +708,22 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -776,22 +806,48 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
         </bottom>
         <vertical/>
         <horizontal style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -811,8 +867,131 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF99FF"/>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FFFF66FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -825,82 +1004,102 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="C12:C16" totalsRowShown="0" headerRowDxfId="36">
-  <autoFilter ref="C12:C16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="C22:C26" totalsRowShown="0" headerRowDxfId="46">
+  <autoFilter ref="C22:C26"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Video" dataDxfId="35"/>
+    <tableColumn id="1" name="Video" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tableau914" displayName="Tableau914" ref="C7:C9" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3" totalsRowBorderDxfId="1">
+  <autoFilter ref="C7:C9"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Genre" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="C6:C10" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
-  <autoFilter ref="C6:C10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="C16:C20" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+  <autoFilter ref="C16:C20"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Image" dataDxfId="30"/>
+    <tableColumn id="1" name="Image" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau7" displayName="Tableau7" ref="C1:C4" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="C1:C4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau7" displayName="Tableau7" ref="A19:A22" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+  <autoFilter ref="A19:A22"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Resource_Category" dataDxfId="25"/>
+    <tableColumn id="1" name="Category_Resource" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau8" displayName="Tableau8" ref="A19:A23" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="A19:A23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau8" displayName="Tableau8" ref="C1:C5" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+  <autoFilter ref="C1:C5"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Resource" dataDxfId="20"/>
+    <tableColumn id="1" name="Resource" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau9" displayName="Tableau9" ref="A15:A17" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau9" displayName="Tableau9" ref="A15:A17" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="A15:A17"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Category" dataDxfId="15"/>
+    <tableColumn id="1" name="Category" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau10" displayName="Tableau10" ref="A10:A13" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau10" displayName="Tableau10" ref="A10:A13" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="A10:A13"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Faq" dataDxfId="10"/>
+    <tableColumn id="1" name="Faq" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tableau11" displayName="Tableau11" ref="A1:A8" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tableau11" displayName="Tableau11" ref="A1:A8" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="A1:A8"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="User" dataDxfId="5"/>
+    <tableColumn id="1" name="User" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau92" displayName="Tableau92" ref="C18:C20" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
-  <autoFilter ref="C18:C20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau92" displayName="Tableau92" ref="A24:A26" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A24:A26"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Role" dataDxfId="0"/>
+    <tableColumn id="1" name="Role" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tableau713" displayName="Tableau713" ref="C11:C14" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="C11:C14"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Genre_Resource" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1167,10 +1366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,14 +1383,14 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1200,146 +1399,173 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>15</v>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
-        <v>25</v>
+      <c r="C9" s="10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>19</v>
+      <c r="C12" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>6</v>
+      <c r="C13" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" s="7" t="s">
-        <v>16</v>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>18</v>
+      <c r="C16" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="C17" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="2" t="s">
-        <v>22</v>
+      <c r="C18" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="C20" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>11</v>
+      <c r="C23" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" orientation="portrait" r:id="rId1"/>
-  <tableParts count="8">
+  <tableParts count="10">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -1348,6 +1574,8 @@
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
NetflixClone doc update -> DB structure
</commit_message>
<xml_diff>
--- a/doc/Table_structure.xlsx
+++ b/doc/Table_structure.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$C$26</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$C$25</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>User</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Resource</t>
   </si>
   <si>
-    <t>category_id</t>
-  </si>
-  <si>
     <t>resource_id</t>
   </si>
   <si>
@@ -113,7 +110,7 @@
     <t>Genre_Resource</t>
   </si>
   <si>
-    <t>Category_Resource</t>
+    <t>category</t>
   </si>
 </sst>
 </file>
@@ -163,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -200,73 +197,173 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="44">
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -301,36 +398,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -347,33 +414,10 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -388,6 +432,13 @@
           <color auto="1"/>
         </top>
         <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
           <color auto="1"/>
         </bottom>
       </border>
@@ -663,6 +714,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <top style="thin">
           <color auto="1"/>
@@ -799,168 +866,6 @@
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="medium">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
@@ -1004,102 +909,92 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="C22:C26" totalsRowShown="0" headerRowDxfId="46">
-  <autoFilter ref="C22:C26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="C21:C25" totalsRowShown="0" headerRowDxfId="43" headerRowBorderDxfId="0" tableBorderDxfId="2">
+  <autoFilter ref="C21:C25"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Video" dataDxfId="45"/>
+    <tableColumn id="1" name="Video" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tableau914" displayName="Tableau914" ref="C7:C9" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3" totalsRowBorderDxfId="1">
-  <autoFilter ref="C7:C9"/>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="A19:A23" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40" totalsRowBorderDxfId="39">
+  <autoFilter ref="A19:A23"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Genre" dataDxfId="4"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="C16:C20" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
-  <autoFilter ref="C16:C20"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Image" dataDxfId="40"/>
+    <tableColumn id="1" name="Image" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau7" displayName="Tableau7" ref="A19:A22" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
-  <autoFilter ref="A19:A22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau8" displayName="Tableau8" ref="C1:C6" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="C1:C6"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Category_Resource" dataDxfId="35"/>
+    <tableColumn id="1" name="Resource" dataDxfId="33"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau9" displayName="Tableau9" ref="C8:C10" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+  <autoFilter ref="C8:C10"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Category" dataDxfId="32"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau10" displayName="Tableau10" ref="A10:A13" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+  <autoFilter ref="A10:A13"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Faq" dataDxfId="27"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tableau11" displayName="Tableau11" ref="A1:A8" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+  <autoFilter ref="A1:A8"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="User" dataDxfId="22"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau92" displayName="Tableau92" ref="A15:A17" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="A15:A17"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Role" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tableau713" displayName="Tableau713" ref="C16:C19" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="C16:C19"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Genre_Resource" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau8" displayName="Tableau8" ref="C1:C5" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
-  <autoFilter ref="C1:C5"/>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tableau914" displayName="Tableau914" ref="C12:C14" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="C12:C14"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Resource" dataDxfId="30"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau9" displayName="Tableau9" ref="A15:A17" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="A15:A17"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Category" dataDxfId="25"/>
+    <tableColumn id="1" name="Genre" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau10" displayName="Tableau10" ref="A10:A13" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="A10:A13"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Faq" dataDxfId="20"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tableau11" displayName="Tableau11" ref="A1:A8" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
-  <autoFilter ref="A1:A8"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="User" dataDxfId="15"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau92" displayName="Tableau92" ref="A24:A26" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A24:A26"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Role" dataDxfId="10"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tableau713" displayName="Tableau713" ref="C11:C14" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
-  <autoFilter ref="C11:C14"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Genre_Resource" dataDxfId="5"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1366,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C25" sqref="A1:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,193 +1274,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="5" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="1" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>17</v>
+      <c r="C25" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" orientation="portrait" r:id="rId1"/>
-  <tableParts count="10">
+  <tableParts count="9">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -1575,7 +1459,6 @@
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
-    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>